<commit_message>
Tables and Figures 2
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\4th_Year\EEE4120F\Prac_2\4120F_Prac2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83673564-8967-41E4-A7DA-D0E2E3DA6ADC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E32AF8-11F3-4741-94F5-62AE676FA5FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF5A649F-1780-4CF6-B272-A8C9F6792F71}"/>
   </bookViews>
@@ -114,13 +114,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,13 +456,13 @@
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="P1" t="s">
         <v>13</v>
       </c>
@@ -622,25 +622,41 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7:I7" si="1">$F$6/G6</f>
+        <v>16.404867043645016</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>26.905065213243141</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>27.599185617913097</v>
+      </c>
       <c r="J7" s="1">
-        <f>F6/J6</f>
+        <f>$F$6/J6</f>
         <v>28.366694789605702</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:M7" si="2">$F$6/K6</f>
+        <v>28.795633061538251</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>21.771084501107744</v>
+      </c>
       <c r="O7" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="2">
         <v>25.227566666666664</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="2">
         <v>7.7489233333333329</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="2">
         <v>4.6553200000000006</v>
       </c>
     </row>
@@ -656,13 +672,13 @@
       <c r="O8" t="s">
         <v>3</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="2">
         <v>9.42544</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="2">
         <v>3.7574933333333331</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="2">
         <v>1.95045</v>
       </c>
     </row>
@@ -692,15 +708,15 @@
       <c r="O9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="2">
         <f>AVERAGE(P7:P8)</f>
         <v>17.326503333333331</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="2">
         <f>AVERAGE(Q7:Q8)</f>
         <v>5.7532083333333333</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="2">
         <f>AVERAGE(R7:R8)</f>
         <v>3.3028850000000003</v>
       </c>
@@ -731,16 +747,16 @@
       <c r="O10" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="2">
         <f>$P$9/P9</f>
         <v>1</v>
       </c>
-      <c r="Q10" s="4">
-        <f t="shared" ref="Q10:R10" si="1">$P$9/Q9</f>
+      <c r="Q10" s="2">
+        <f t="shared" ref="Q10:R10" si="3">$P$9/Q9</f>
         <v>3.0116245283428809</v>
       </c>
-      <c r="R10" s="4">
-        <f t="shared" si="1"/>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
         <v>5.2458693939793033</v>
       </c>
     </row>
@@ -775,11 +791,11 @@
         <v>25.227566666666664</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:D12" si="2">AVERAGE(C9:C11)</f>
+        <f t="shared" ref="C12:D12" si="4">AVERAGE(C9:C11)</f>
         <v>7.7489233333333329</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.6553200000000006</v>
       </c>
       <c r="F12" s="1">
@@ -790,7 +806,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1">
-        <f t="shared" ref="G12:J12" si="3">AVERAGE(J9:J11)</f>
+        <f t="shared" ref="J12" si="5">AVERAGE(J9:J11)</f>
         <v>0.72345766666666655</v>
       </c>
       <c r="L12">
@@ -894,11 +910,11 @@
         <v>9.42544</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:D20" si="4">AVERAGE(C17:C19)</f>
+        <f t="shared" ref="C20:D20" si="6">AVERAGE(C17:C19)</f>
         <v>3.7574933333333331</v>
       </c>
       <c r="D20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.95045</v>
       </c>
       <c r="F20" s="1"/>
@@ -913,11 +929,11 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:D21" si="5">$B$20/C20</f>
+        <f t="shared" ref="C21:D21" si="7">$B$20/C20</f>
         <v>2.5084382496132176</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.8324437950216614</v>
       </c>
       <c r="F21" s="1"/>
@@ -980,7 +996,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1">
-        <f t="shared" ref="J27" si="6">AVERAGE(J24:J26)</f>
+        <f t="shared" ref="J27" si="8">AVERAGE(J24:J26)</f>
         <v>3.8695233333333329E-2</v>
       </c>
     </row>
@@ -1058,5 +1074,6 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Tables and Figures 2"
This reverts commit 0e142d418835c7f471aa7a1bfc3242018f8b3489.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\4th_Year\EEE4120F\Prac_2\4120F_Prac2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E32AF8-11F3-4741-94F5-62AE676FA5FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83673564-8967-41E4-A7DA-D0E2E3DA6ADC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF5A649F-1780-4CF6-B272-A8C9F6792F71}"/>
   </bookViews>
@@ -114,13 +114,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,13 +456,13 @@
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
       <c r="P1" t="s">
         <v>13</v>
       </c>
@@ -622,41 +622,25 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>
-      <c r="G7" s="1">
-        <f t="shared" ref="G7:I7" si="1">$F$6/G6</f>
-        <v>16.404867043645016</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>26.905065213243141</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="1"/>
-        <v>27.599185617913097</v>
-      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1">
-        <f>$F$6/J6</f>
+        <f>F6/J6</f>
         <v>28.366694789605702</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" ref="K7:M7" si="2">$F$6/K6</f>
-        <v>28.795633061538251</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
-        <f t="shared" si="2"/>
-        <v>21.771084501107744</v>
-      </c>
+      <c r="K7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="O7" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="4">
         <v>25.227566666666664</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="4">
         <v>7.7489233333333329</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="4">
         <v>4.6553200000000006</v>
       </c>
     </row>
@@ -672,13 +656,13 @@
       <c r="O8" t="s">
         <v>3</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="4">
         <v>9.42544</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="4">
         <v>3.7574933333333331</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="4">
         <v>1.95045</v>
       </c>
     </row>
@@ -708,15 +692,15 @@
       <c r="O9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="4">
         <f>AVERAGE(P7:P8)</f>
         <v>17.326503333333331</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="4">
         <f>AVERAGE(Q7:Q8)</f>
         <v>5.7532083333333333</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="4">
         <f>AVERAGE(R7:R8)</f>
         <v>3.3028850000000003</v>
       </c>
@@ -747,16 +731,16 @@
       <c r="O10" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="4">
         <f>$P$9/P9</f>
         <v>1</v>
       </c>
-      <c r="Q10" s="2">
-        <f t="shared" ref="Q10:R10" si="3">$P$9/Q9</f>
+      <c r="Q10" s="4">
+        <f t="shared" ref="Q10:R10" si="1">$P$9/Q9</f>
         <v>3.0116245283428809</v>
       </c>
-      <c r="R10" s="2">
-        <f t="shared" si="3"/>
+      <c r="R10" s="4">
+        <f t="shared" si="1"/>
         <v>5.2458693939793033</v>
       </c>
     </row>
@@ -791,11 +775,11 @@
         <v>25.227566666666664</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:D12" si="4">AVERAGE(C9:C11)</f>
+        <f t="shared" ref="C12:D12" si="2">AVERAGE(C9:C11)</f>
         <v>7.7489233333333329</v>
       </c>
       <c r="D12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4.6553200000000006</v>
       </c>
       <c r="F12" s="1">
@@ -806,7 +790,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1">
-        <f t="shared" ref="J12" si="5">AVERAGE(J9:J11)</f>
+        <f t="shared" ref="G12:J12" si="3">AVERAGE(J9:J11)</f>
         <v>0.72345766666666655</v>
       </c>
       <c r="L12">
@@ -910,11 +894,11 @@
         <v>9.42544</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:D20" si="6">AVERAGE(C17:C19)</f>
+        <f t="shared" ref="C20:D20" si="4">AVERAGE(C17:C19)</f>
         <v>3.7574933333333331</v>
       </c>
       <c r="D20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.95045</v>
       </c>
       <c r="F20" s="1"/>
@@ -929,11 +913,11 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:D21" si="7">$B$20/C20</f>
+        <f t="shared" ref="C21:D21" si="5">$B$20/C20</f>
         <v>2.5084382496132176</v>
       </c>
       <c r="D21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4.8324437950216614</v>
       </c>
       <c r="F21" s="1"/>
@@ -996,7 +980,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1">
-        <f t="shared" ref="J27" si="8">AVERAGE(J24:J26)</f>
+        <f t="shared" ref="J27" si="6">AVERAGE(J24:J26)</f>
         <v>3.8695233333333329E-2</v>
       </c>
     </row>
@@ -1074,6 +1058,5 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>